<commit_message>
UML en XSD bijgewerkt
</commit_message>
<xml_diff>
--- a/uml/IMKL2.x/IMKL-changelog.xlsx
+++ b/uml/IMKL2.x/IMKL-changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-dev\uml\IMKL2.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB22C213-342A-4B27-8408-819CA817CC83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C560013-6D7C-4764-AC80-1D12202AEBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
+    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>Datum</t>
   </si>
@@ -114,9 +114,6 @@
     <t>locatieWerkzaamheden</t>
   </si>
   <si>
-    <t>ChracaterString -&gt; Adres</t>
-  </si>
-  <si>
     <t>definitie aangepast</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>voorbereidingMedegebruikFysiekeInfrastructuur</t>
   </si>
   <si>
-    <t>toegevoegd, definitie?</t>
-  </si>
-  <si>
     <t>bestandMediaType</t>
   </si>
   <si>
@@ -238,6 +232,36 @@
   </si>
   <si>
     <t>Max1AlgemeneBijlage</t>
+  </si>
+  <si>
+    <t>KabelOfLeiding</t>
+  </si>
+  <si>
+    <t>Maximaal1Utiliteitsnet</t>
+  </si>
+  <si>
+    <t>inNetwork</t>
+  </si>
+  <si>
+    <t>KabelEnLeidingContainer</t>
+  </si>
+  <si>
+    <t>KaartBGTbestandVerplicht</t>
+  </si>
+  <si>
+    <t>Moet herschreven</t>
+  </si>
+  <si>
+    <t>GebiedInformatieLevering: OPMERKING: Controleer</t>
+  </si>
+  <si>
+    <t>XSD</t>
+  </si>
+  <si>
+    <t>CharacterString -&gt; Adres</t>
+  </si>
+  <si>
+    <t>toegevoegd plus definitie</t>
   </si>
 </sst>
 </file>
@@ -674,11 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B8AAF5-2631-4C35-B121-F1562B5D065D}">
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:M181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -689,11 +713,12 @@
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" customWidth="1"/>
     <col min="6" max="6" width="47.42578125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,12 +737,15 @@
       <c r="F1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>43943</v>
       </c>
@@ -730,14 +758,17 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="11">
+        <v>58</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="11">
         <v>240</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>43943</v>
       </c>
@@ -752,12 +783,13 @@
       <c r="F3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="15"/>
+      <c r="H3" s="11">
         <v>240</v>
       </c>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>43943</v>
       </c>
@@ -772,12 +804,15 @@
       <c r="F4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="11">
         <v>280</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>43943</v>
       </c>
@@ -792,12 +827,15 @@
       <c r="F5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="11">
         <v>210</v>
       </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>43943</v>
       </c>
@@ -812,12 +850,15 @@
       <c r="F6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="11">
         <v>210</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>43943</v>
       </c>
@@ -832,12 +873,13 @@
       <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="15"/>
+      <c r="H7" s="11">
         <v>210</v>
       </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>43943</v>
       </c>
@@ -852,12 +894,15 @@
       <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="11">
         <v>210</v>
       </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>43943</v>
       </c>
@@ -872,12 +917,13 @@
       <c r="F9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="15"/>
+      <c r="H9" s="11">
         <v>210</v>
       </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>43943</v>
       </c>
@@ -894,12 +940,13 @@
       <c r="F10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="15"/>
+      <c r="H10" s="11">
         <v>239</v>
       </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>43943</v>
       </c>
@@ -912,14 +959,17 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="11">
+        <v>74</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="11">
         <v>219</v>
       </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>43943</v>
       </c>
@@ -932,14 +982,17 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="11">
+        <v>26</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="11">
         <v>219</v>
       </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>43943</v>
       </c>
@@ -947,41 +1000,47 @@
         <v>24</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="11">
         <v>219</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I13" s="7"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>43943</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="11">
+        <v>30</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="11">
         <v>215</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I14" s="6"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>43943</v>
       </c>
@@ -991,18 +1050,19 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="G15" s="16"/>
+      <c r="H15" s="11">
         <v>214</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I15" s="6"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>43943</v>
       </c>
@@ -1010,20 +1070,23 @@
         <v>24</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="11">
+        <v>75</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="11">
         <v>199</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="6"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>43943</v>
       </c>
@@ -1031,1854 +1094,2061 @@
         <v>24</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="11">
+        <v>75</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="11">
         <v>199</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I17" s="7"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>43943</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="11">
-        <v>195</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="11">
+        <v>197</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>43943</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="11">
+        <v>30</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="11">
         <v>197</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I19" s="6"/>
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>43943</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="16"/>
+      <c r="H20" s="11">
         <v>195</v>
       </c>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>43943</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="11">
+        <v>39</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="11">
         <v>193</v>
       </c>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>43943</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="11">
+        <v>43</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="11">
         <v>195</v>
       </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>43943</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="11">
+        <v>43</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="11">
         <v>282</v>
       </c>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>43944</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="11">
+        <v>57</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="11">
         <v>215</v>
       </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" ht="72" x14ac:dyDescent="0.2">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" ht="72" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>43959</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="11">
+        <v>59</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="11">
         <v>215</v>
       </c>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>43959</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="11">
+        <v>61</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="11">
         <v>286</v>
       </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>43959</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
+        <v>43973</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="11">
+        <v>269</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
+        <v>43973</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E31" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="11">
+        <v>269</v>
+      </c>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="16"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G32" s="16"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G34" s="16"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="16"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G35" s="16"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="16"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G36" s="16"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="16"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G37" s="16"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="16"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G38" s="16"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="16"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="6"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G39" s="16"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G40" s="16"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G41" s="16"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="16"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G42" s="16"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="16"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="6"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G43" s="16"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="16"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="6"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G44" s="16"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="6"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G45" s="16"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="16"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G46" s="16"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="16"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="6"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G47" s="16"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="16"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G48" s="16"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="16"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G49" s="16"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="16"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="6"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G50" s="16"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="16"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G51" s="16"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="16"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G52" s="16"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="16"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="6"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G53" s="16"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="16"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="6"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G54" s="16"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="16"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G55" s="16"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="16"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G56" s="16"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="16"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G57" s="16"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="16"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G58" s="16"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="16"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G59" s="16"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="16"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="3"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="6"/>
       <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="16"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="3"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="6"/>
       <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="16"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="3"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="6"/>
       <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="16"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="3"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="6"/>
       <c r="J63" s="3"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="16"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="3"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="6"/>
       <c r="J64" s="3"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K64" s="3"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="7"/>
-      <c r="I65" s="3"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="7"/>
       <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="16"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="3"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="7"/>
       <c r="J66" s="3"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K66" s="3"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="16"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="3"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="6"/>
       <c r="J67" s="3"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="3"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="6"/>
       <c r="J68" s="3"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K68" s="3"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="17"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="7"/>
-      <c r="I69" s="3"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="7"/>
       <c r="J69" s="3"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="17"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="3"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="7"/>
       <c r="J70" s="3"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
       <c r="F71" s="17"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="3"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="6"/>
       <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
       <c r="F72" s="17"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="3"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="6"/>
       <c r="J72" s="3"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K72" s="3"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="7"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
       <c r="F73" s="17"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="3"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="6"/>
       <c r="J73" s="3"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="7"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
       <c r="F74" s="17"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="3"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="6"/>
       <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K74" s="3"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="17"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="3"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="6"/>
       <c r="J75" s="3"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="17"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="3"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="6"/>
       <c r="J76" s="3"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K76" s="3"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="17"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="6"/>
-      <c r="I77" s="3"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="6"/>
       <c r="J77" s="3"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="17"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="6"/>
-      <c r="I78" s="3"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="6"/>
       <c r="J78" s="3"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
       <c r="F79" s="17"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="6"/>
-      <c r="I79" s="3"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="6"/>
       <c r="J79" s="3"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
       <c r="F80" s="17"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="3"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="6"/>
       <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="17"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="3"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="6"/>
       <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="17"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="6"/>
-      <c r="I82" s="3"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="6"/>
       <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K82" s="3"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="17"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="6"/>
-      <c r="I83" s="3"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="11"/>
+      <c r="I83" s="6"/>
       <c r="J83" s="3"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="F84" s="17"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="3"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="6"/>
       <c r="J84" s="3"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K84" s="3"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="17"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="6"/>
-      <c r="I85" s="3"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="11"/>
+      <c r="I85" s="6"/>
       <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K85" s="3"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="F86" s="17"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="3"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="6"/>
       <c r="J86" s="3"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K86" s="3"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6"/>
       <c r="F87" s="17"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="3"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="6"/>
       <c r="J87" s="3"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K87" s="3"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6"/>
       <c r="F88" s="17"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="7"/>
-      <c r="I88" s="3"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="7"/>
       <c r="J88" s="3"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K88" s="3"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6"/>
       <c r="F89" s="17"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="7"/>
-      <c r="I89" s="3"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="7"/>
       <c r="J89" s="3"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6"/>
       <c r="F90" s="17"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="7"/>
-      <c r="I90" s="3"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="7"/>
       <c r="J90" s="3"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K90" s="3"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="F91" s="17"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="3"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="7"/>
       <c r="J91" s="3"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
       <c r="F92" s="17"/>
-      <c r="G92" s="11"/>
-      <c r="H92" s="7"/>
-      <c r="I92" s="3"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="7"/>
       <c r="J92" s="3"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K92" s="3"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
       <c r="E93" s="6"/>
       <c r="F93" s="17"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="3"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="7"/>
       <c r="J93" s="3"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
       <c r="F94" s="17"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="3"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="6"/>
       <c r="J94" s="3"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K94" s="3"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="7"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="6"/>
       <c r="F95" s="17"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="3"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="6"/>
       <c r="J95" s="3"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="7"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="6"/>
       <c r="F96" s="17"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="3"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="6"/>
       <c r="J96" s="3"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K96" s="3"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="7"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="F97" s="17"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="3"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="6"/>
       <c r="J97" s="3"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="F98" s="17"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="3"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="6"/>
       <c r="J98" s="3"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K98" s="3"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
       <c r="F99" s="17"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="6"/>
-      <c r="I99" s="3"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="6"/>
       <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
       <c r="F100" s="17"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="6"/>
-      <c r="I100" s="3"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="6"/>
       <c r="J100" s="3"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K100" s="3"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
       <c r="F101" s="17"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="3"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="6"/>
       <c r="J101" s="3"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
       <c r="F102" s="17"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="3"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="11"/>
+      <c r="I102" s="6"/>
       <c r="J102" s="3"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
       <c r="F103" s="17"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="3"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="6"/>
       <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
       <c r="F104" s="17"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="3"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="6"/>
       <c r="J104" s="3"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K104" s="3"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
       <c r="F105" s="17"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="3"/>
+      <c r="G105" s="17"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="6"/>
       <c r="J105" s="3"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
       <c r="F106" s="17"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="6"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G106" s="17"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="6"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
       <c r="F107" s="17"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="6"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G107" s="17"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="6"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
       <c r="F108" s="17"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="6"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G108" s="17"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="6"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
       <c r="F109" s="17"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="6"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G109" s="17"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="6"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
       <c r="F110" s="17"/>
-      <c r="G110" s="11"/>
-      <c r="H110" s="6"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G110" s="17"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="6"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
       <c r="F111" s="17"/>
-      <c r="G111" s="11"/>
-      <c r="H111" s="6"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G111" s="17"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="6"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
       <c r="F112" s="17"/>
-      <c r="G112" s="11"/>
-      <c r="H112" s="6"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G112" s="17"/>
+      <c r="H112" s="11"/>
+      <c r="I112" s="6"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
       <c r="F113" s="17"/>
-      <c r="G113" s="11"/>
-      <c r="H113" s="6"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G113" s="17"/>
+      <c r="H113" s="11"/>
+      <c r="I113" s="6"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
       <c r="F114" s="17"/>
-      <c r="G114" s="11"/>
-      <c r="H114" s="6"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G114" s="17"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="6"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
       <c r="F115" s="17"/>
-      <c r="G115" s="11"/>
-      <c r="H115" s="6"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G115" s="17"/>
+      <c r="H115" s="11"/>
+      <c r="I115" s="6"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
       <c r="F116" s="17"/>
-      <c r="G116" s="11"/>
-      <c r="H116" s="6"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G116" s="17"/>
+      <c r="H116" s="11"/>
+      <c r="I116" s="6"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
       <c r="F117" s="17"/>
-      <c r="G117" s="11"/>
-      <c r="H117" s="6"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G117" s="17"/>
+      <c r="H117" s="11"/>
+      <c r="I117" s="6"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
       <c r="F118" s="17"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="6"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G118" s="17"/>
+      <c r="H118" s="11"/>
+      <c r="I118" s="6"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
       <c r="F119" s="17"/>
-      <c r="G119" s="11"/>
-      <c r="H119" s="6"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G119" s="17"/>
+      <c r="H119" s="11"/>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
       <c r="F120" s="17"/>
-      <c r="G120" s="11"/>
-      <c r="H120" s="6"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G120" s="17"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="6"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
       <c r="F121" s="17"/>
-      <c r="G121" s="11"/>
-      <c r="H121" s="6"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G121" s="17"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="6"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
       <c r="E122" s="6"/>
       <c r="F122" s="17"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="6"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G122" s="17"/>
+      <c r="H122" s="11"/>
+      <c r="I122" s="6"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="6"/>
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
       <c r="F123" s="17"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="6"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G123" s="17"/>
+      <c r="H123" s="11"/>
+      <c r="I123" s="6"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="7"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
       <c r="E124" s="6"/>
       <c r="F124" s="17"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="6"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G124" s="17"/>
+      <c r="H124" s="11"/>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="6"/>
       <c r="E125" s="6"/>
       <c r="F125" s="17"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="6"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G125" s="17"/>
+      <c r="H125" s="11"/>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
       <c r="D126" s="6"/>
       <c r="E126" s="6"/>
       <c r="F126" s="17"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="6"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G126" s="17"/>
+      <c r="H126" s="11"/>
+      <c r="I126" s="6"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="7"/>
       <c r="F127" s="16"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="7"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G127" s="16"/>
+      <c r="H127" s="11"/>
+      <c r="I127" s="7"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="7"/>
       <c r="F128" s="16"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="7"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G128" s="16"/>
+      <c r="H128" s="11"/>
+      <c r="I128" s="7"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="7"/>
       <c r="F129" s="16"/>
-      <c r="G129" s="11"/>
-      <c r="H129" s="7"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G129" s="16"/>
+      <c r="H129" s="11"/>
+      <c r="I129" s="7"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="5"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
       <c r="F130" s="18"/>
-      <c r="G130" s="11"/>
-      <c r="H130" s="4"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G130" s="18"/>
+      <c r="H130" s="11"/>
+      <c r="I130" s="4"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="5"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
       <c r="F131" s="18"/>
-      <c r="G131" s="11"/>
-      <c r="H131" s="4"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G131" s="18"/>
+      <c r="H131" s="11"/>
+      <c r="I131" s="4"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="5"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
       <c r="F132" s="18"/>
-      <c r="G132" s="11"/>
-      <c r="H132" s="4"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G132" s="18"/>
+      <c r="H132" s="11"/>
+      <c r="I132" s="4"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="5"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
       <c r="F133" s="18"/>
-      <c r="G133" s="11"/>
-      <c r="H133" s="4"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G133" s="18"/>
+      <c r="H133" s="11"/>
+      <c r="I133" s="4"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="5"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
       <c r="F134" s="18"/>
-      <c r="G134" s="11"/>
-      <c r="H134" s="4"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G134" s="18"/>
+      <c r="H134" s="11"/>
+      <c r="I134" s="4"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="5"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="18"/>
-      <c r="G135" s="11"/>
-      <c r="H135" s="4"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G135" s="18"/>
+      <c r="H135" s="11"/>
+      <c r="I135" s="4"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="5"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="18"/>
-      <c r="G136" s="11"/>
-      <c r="H136" s="4"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G136" s="18"/>
+      <c r="H136" s="11"/>
+      <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="5"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="F137" s="18"/>
-      <c r="G137" s="11"/>
-      <c r="H137" s="4"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G137" s="18"/>
+      <c r="H137" s="11"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
       <c r="F138" s="18"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="4"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G138" s="18"/>
+      <c r="H138" s="12"/>
+      <c r="I138" s="4"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
       <c r="F139" s="18"/>
-      <c r="G139" s="12"/>
-      <c r="H139" s="4"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G139" s="18"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
       <c r="F140" s="18"/>
-      <c r="G140" s="12"/>
-      <c r="H140" s="4"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G140" s="18"/>
+      <c r="H140" s="12"/>
+      <c r="I140" s="4"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
       <c r="F141" s="18"/>
-      <c r="G141" s="12"/>
-      <c r="H141" s="4"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G141" s="18"/>
+      <c r="H141" s="12"/>
+      <c r="I141" s="4"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
       <c r="F142" s="18"/>
-      <c r="G142" s="12"/>
-      <c r="H142" s="4"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G142" s="18"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="4"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
       <c r="F143" s="18"/>
-      <c r="G143" s="12"/>
-      <c r="H143" s="4"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G143" s="18"/>
+      <c r="H143" s="12"/>
+      <c r="I143" s="4"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
       <c r="F144" s="18"/>
-      <c r="G144" s="12"/>
-      <c r="H144" s="4"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G144" s="18"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="4"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
       <c r="F145" s="18"/>
-      <c r="G145" s="12"/>
-      <c r="H145" s="4"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G145" s="18"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="4"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
       <c r="F146" s="18"/>
-      <c r="G146" s="12"/>
-      <c r="H146" s="4"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G146" s="18"/>
+      <c r="H146" s="12"/>
+      <c r="I146" s="4"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
       <c r="F147" s="18"/>
-      <c r="G147" s="12"/>
-      <c r="H147" s="4"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G147" s="18"/>
+      <c r="H147" s="12"/>
+      <c r="I147" s="4"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
       <c r="F148" s="18"/>
-      <c r="G148" s="12"/>
-      <c r="H148" s="4"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G148" s="18"/>
+      <c r="H148" s="12"/>
+      <c r="I148" s="4"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
       <c r="F149" s="18"/>
-      <c r="G149" s="12"/>
-      <c r="H149" s="4"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G149" s="18"/>
+      <c r="H149" s="12"/>
+      <c r="I149" s="4"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="4"/>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
       <c r="F150" s="18"/>
-      <c r="G150" s="12"/>
-      <c r="H150" s="4"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G150" s="18"/>
+      <c r="H150" s="12"/>
+      <c r="I150" s="4"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="4"/>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="18"/>
-      <c r="G151" s="12"/>
-      <c r="H151" s="4"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G151" s="18"/>
+      <c r="H151" s="12"/>
+      <c r="I151" s="4"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
       <c r="F152" s="18"/>
-      <c r="G152" s="12"/>
-      <c r="H152" s="4"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G152" s="18"/>
+      <c r="H152" s="12"/>
+      <c r="I152" s="4"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
       <c r="F153" s="18"/>
-      <c r="G153" s="12"/>
-      <c r="H153" s="4"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G153" s="18"/>
+      <c r="H153" s="12"/>
+      <c r="I153" s="4"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="4"/>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
       <c r="F154" s="18"/>
-      <c r="G154" s="12"/>
-      <c r="H154" s="4"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G154" s="18"/>
+      <c r="H154" s="12"/>
+      <c r="I154" s="4"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="4"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
       <c r="F155" s="18"/>
-      <c r="G155" s="12"/>
-      <c r="H155" s="4"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G155" s="18"/>
+      <c r="H155" s="12"/>
+      <c r="I155" s="4"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="4"/>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
       <c r="F156" s="18"/>
-      <c r="G156" s="12"/>
-      <c r="H156" s="4"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G156" s="18"/>
+      <c r="H156" s="12"/>
+      <c r="I156" s="4"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="4"/>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
       <c r="F157" s="18"/>
-      <c r="G157" s="12"/>
-      <c r="H157" s="4"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G157" s="18"/>
+      <c r="H157" s="12"/>
+      <c r="I157" s="4"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="4"/>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
       <c r="F158" s="18"/>
-      <c r="G158" s="12"/>
-      <c r="H158" s="4"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G158" s="18"/>
+      <c r="H158" s="12"/>
+      <c r="I158" s="4"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="4"/>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
       <c r="F159" s="18"/>
-      <c r="G159" s="12"/>
-      <c r="H159" s="4"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G159" s="18"/>
+      <c r="H159" s="12"/>
+      <c r="I159" s="4"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="4"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
       <c r="F160" s="18"/>
-      <c r="G160" s="12"/>
-      <c r="H160" s="4"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G160" s="18"/>
+      <c r="H160" s="12"/>
+      <c r="I160" s="4"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="4"/>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
       <c r="F161" s="18"/>
-      <c r="G161" s="12"/>
-      <c r="H161" s="4"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G161" s="18"/>
+      <c r="H161" s="12"/>
+      <c r="I161" s="4"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="4"/>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
       <c r="F162" s="18"/>
-      <c r="G162" s="12"/>
-      <c r="H162" s="4"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G162" s="18"/>
+      <c r="H162" s="12"/>
+      <c r="I162" s="4"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="4"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
       <c r="F163" s="18"/>
-      <c r="G163" s="12"/>
-      <c r="H163" s="4"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G163" s="18"/>
+      <c r="H163" s="12"/>
+      <c r="I163" s="4"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="4"/>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
       <c r="F164" s="18"/>
-      <c r="G164" s="12"/>
-      <c r="H164" s="4"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G164" s="18"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="4"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="4"/>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
       <c r="F165" s="18"/>
-      <c r="G165" s="12"/>
-      <c r="H165" s="4"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G165" s="18"/>
+      <c r="H165" s="12"/>
+      <c r="I165" s="4"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="4"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
       <c r="F166" s="18"/>
-      <c r="G166" s="12"/>
-      <c r="H166" s="4"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G166" s="18"/>
+      <c r="H166" s="12"/>
+      <c r="I166" s="4"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="4"/>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
       <c r="F167" s="18"/>
-      <c r="G167" s="12"/>
-      <c r="H167" s="4"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G167" s="18"/>
+      <c r="H167" s="12"/>
+      <c r="I167" s="4"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="4"/>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
       <c r="F168" s="18"/>
-      <c r="G168" s="12"/>
-      <c r="H168" s="4"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G168" s="18"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="4"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="4"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
       <c r="F169" s="18"/>
-      <c r="G169" s="12"/>
-      <c r="H169" s="4"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G169" s="18"/>
+      <c r="H169" s="12"/>
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="4"/>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
       <c r="F170" s="18"/>
-      <c r="G170" s="12"/>
-      <c r="H170" s="4"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G170" s="18"/>
+      <c r="H170" s="12"/>
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="4"/>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
       <c r="F171" s="18"/>
-      <c r="G171" s="12"/>
-      <c r="H171" s="4"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G171" s="18"/>
+      <c r="H171" s="12"/>
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="4"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
       <c r="F172" s="18"/>
-      <c r="G172" s="12"/>
-      <c r="H172" s="4"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G172" s="18"/>
+      <c r="H172" s="12"/>
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="4"/>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
       <c r="F173" s="18"/>
-      <c r="G173" s="12"/>
-      <c r="H173" s="4"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G173" s="18"/>
+      <c r="H173" s="12"/>
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="4"/>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
       <c r="F174" s="18"/>
-      <c r="G174" s="12"/>
-      <c r="H174" s="4"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G174" s="18"/>
+      <c r="H174" s="12"/>
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="4"/>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
       <c r="F175" s="18"/>
-      <c r="G175" s="12"/>
-      <c r="H175" s="4"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G175" s="18"/>
+      <c r="H175" s="12"/>
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="4"/>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
       <c r="F176" s="18"/>
-      <c r="G176" s="12"/>
-      <c r="H176" s="4"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G176" s="18"/>
+      <c r="H176" s="12"/>
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="4"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
       <c r="F177" s="18"/>
-      <c r="G177" s="12"/>
-      <c r="H177" s="4"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G177" s="18"/>
+      <c r="H177" s="12"/>
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="4"/>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
       <c r="F178" s="18"/>
-      <c r="G178" s="12"/>
-      <c r="H178" s="4"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G178" s="18"/>
+      <c r="H178" s="12"/>
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="4"/>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
       <c r="F179" s="18"/>
-      <c r="G179" s="12"/>
-      <c r="H179" s="4"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G179" s="18"/>
+      <c r="H179" s="12"/>
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="4"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
       <c r="F180" s="18"/>
-      <c r="G180" s="12"/>
-      <c r="H180" s="4"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G180" s="18"/>
+      <c r="H180" s="12"/>
+      <c r="I180" s="4"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="4"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
       <c r="F181" s="18"/>
-      <c r="G181" s="12"/>
-      <c r="H181" s="4"/>
+      <c r="G181" s="18"/>
+      <c r="H181" s="12"/>
+      <c r="I181" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2907,7 +3177,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2915,36 +3185,36 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>51</v>
-      </c>
       <c r="H3" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
         <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3156,18 +3426,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3190,18 +3460,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>